<commit_message>
Update excel path to config file
</commit_message>
<xml_diff>
--- a/GUI/App_Data/Excel_File/FileTest.xlsx
+++ b/GUI/App_Data/Excel_File/FileTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\Programing\OceanTeach_Net_L1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\Programing\OceanTeach_Net_L1\20230104_DangQuangTrung_L2\EmployeeManager\GUI\App_Data\Excel_File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379986FF-528E-487E-997A-D639F2FC1EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C07097-369C-49DB-BAAD-33F4461F67BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Tên Employee</t>
   </si>
@@ -51,19 +51,16 @@
     <t>Cụ thể</t>
   </si>
   <si>
-    <t>Duc</t>
-  </si>
-  <si>
     <t>121231231233</t>
   </si>
   <si>
-    <t>0123456789</t>
-  </si>
-  <si>
     <t>Mã dân tộc</t>
   </si>
   <si>
     <t>Mã công việc</t>
+  </si>
+  <si>
+    <t>Duc Mạnh</t>
   </si>
 </sst>
 </file>
@@ -414,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -467,7 +464,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5">
         <v>36527</v>
@@ -479,11 +476,9 @@
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F2" s="6"/>
       <c r="G2">
         <v>3</v>
       </c>
@@ -496,6 +491,38 @@
       <c r="J2">
         <v>312</v>
       </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="5">
+        <v>36527</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
move db model to dto
</commit_message>
<xml_diff>
--- a/GUI/App_Data/Excel_File/FileTest.xlsx
+++ b/GUI/App_Data/Excel_File/FileTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\Programing\OceanTeach_Net_L1\20230104_DangQuangTrung_L2\EmployeeManager\GUI\App_Data\Excel_File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C07097-369C-49DB-BAAD-33F4461F67BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D479F7A-8247-4EF2-A2F3-5B01E2C9E6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Tên Employee</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Duc Mạnh</t>
+  </si>
+  <si>
+    <t>0962772733</t>
+  </si>
+  <si>
+    <t>Trung</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,7 +484,9 @@
       <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G2">
         <v>3</v>
       </c>
@@ -493,6 +501,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
       <c r="B3" s="5">
         <v>36527</v>
       </c>
@@ -505,7 +516,9 @@
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="G3">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
add view model to all models correct error in db
</commit_message>
<xml_diff>
--- a/GUI/App_Data/Excel_File/FileTest.xlsx
+++ b/GUI/App_Data/Excel_File/FileTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive\Documents\Programing\OceanTeach_Net_L1\20230104_DangQuangTrung_L2\EmployeeManager\GUI\App_Data\Excel_File\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EmployeeManager\GUI\App_Data\Excel_File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D479F7A-8247-4EF2-A2F3-5B01E2C9E6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5CC6B4-ED7C-4EDB-8033-D497384C7074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -420,7 +420,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,7 +488,7 @@
         <v>12</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -520,10 +520,10 @@
         <v>12</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>31313</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="I3">
         <v>3</v>

</xml_diff>